<commit_message>
added last CS folderwith 870 CS files
</commit_message>
<xml_diff>
--- a/saybapco/CS_OLD2/000-A-PRI-50009-001-RA-CS.xlsx
+++ b/saybapco/CS_OLD2/000-A-PRI-50009-001-RA-CS.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LocalData\076551C-BAPCO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LocalData\076551C-BAPCO\CS SISTEMATI\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1184,7 +1184,7 @@
   <dimension ref="A1:H90"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>